<commit_message>
Adding LaTeX files for write-up
</commit_message>
<xml_diff>
--- a/2/Report/report_data.xlsx
+++ b/2/Report/report_data.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet3!$F$21:$G$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet3!$F$22:$G$22</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
@@ -9674,9 +9674,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="58">
+  <cellStyleXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -9783,7 +9805,7 @@
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="58">
+  <cellStyles count="80">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -9812,6 +9834,17 @@
     <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -9840,6 +9873,17 @@
     <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -10636,47 +10680,47 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet3!$F$22:$F$26</c:f>
+              <c:f>Sheet3!$F$23:$F$27</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>All calls</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>All calls + Arguments</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>All calls + Arguments + First calls + Bigrams</c:v>
+                <c:pt idx="2">
+                  <c:v>All calls + Arguments + First calls</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>All calls +Bigrams</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>All calls</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>All calls + Arguments + First calls</c:v>
+                  <c:v>All calls + Arguments + First calls + Bigrams</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$G$22:$G$26</c:f>
+              <c:f>Sheet3!$G$23:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
+                  <c:v>0.8894137</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.876221</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.886731</c:v>
+                <c:pt idx="2">
+                  <c:v>0.900651</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.88835</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.8894137</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.900651</c:v>
+                  <c:v>0.886731</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10836,16 +10880,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10866,16 +10910,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>468114</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -59038,10 +59082,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -59167,7 +59211,7 @@
         <v>0.84201999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>3121</v>
       </c>
@@ -59175,7 +59219,7 @@
         <v>0.86150000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>3124</v>
       </c>
@@ -59183,7 +59227,7 @@
         <v>0.86807800000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>3117</v>
       </c>
@@ -59191,19 +59235,16 @@
         <v>0.87622100000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:9">
       <c r="B20" s="28"/>
-      <c r="F20" t="s">
-        <v>3117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="27" t="s">
         <v>3127</v>
       </c>
       <c r="B21" s="28"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>3122</v>
       </c>
@@ -59211,13 +59252,10 @@
         <v>3123</v>
       </c>
       <c r="F22" t="s">
-        <v>3131</v>
-      </c>
-      <c r="G22" s="30">
-        <v>0.87622100000000003</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>3117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>3118</v>
       </c>
@@ -59225,13 +59263,13 @@
         <v>0.42182399999999998</v>
       </c>
       <c r="F23" t="s">
-        <v>3135</v>
+        <v>3130</v>
       </c>
       <c r="G23" s="30">
-        <v>0.88673100000000005</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>0.88941369999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>3120</v>
       </c>
@@ -59239,13 +59277,13 @@
         <v>0.76221499999999998</v>
       </c>
       <c r="F24" t="s">
-        <v>3134</v>
+        <v>3131</v>
       </c>
       <c r="G24" s="30">
-        <v>0.88834999999999997</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>0.87622100000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>3116</v>
       </c>
@@ -59253,13 +59291,17 @@
         <v>0.80618690000000004</v>
       </c>
       <c r="F25" t="s">
-        <v>3130</v>
+        <v>3132</v>
       </c>
       <c r="G25" s="30">
-        <v>0.88941369999999997</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>0.90065099999999998</v>
+      </c>
+      <c r="H25" s="30">
+        <f>G25-G23</f>
+        <v>1.1237300000000006E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>3119</v>
       </c>
@@ -59267,21 +59309,28 @@
         <v>0.83224799999999999</v>
       </c>
       <c r="F26" t="s">
-        <v>3132</v>
+        <v>3134</v>
       </c>
       <c r="G26" s="30">
-        <v>0.90065099999999998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>0.88834999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>3121</v>
       </c>
       <c r="B27" s="28">
         <v>0.861564</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="F27" t="s">
+        <v>3135</v>
+      </c>
+      <c r="G27" s="30">
+        <v>0.88673100000000005</v>
+      </c>
+      <c r="I27" s="30"/>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>3124</v>
       </c>
@@ -59289,7 +59338,7 @@
         <v>0.87785000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>3117</v>
       </c>
@@ -59297,16 +59346,16 @@
         <v>0.89739400000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:9">
       <c r="B30" s="28"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:9">
       <c r="A31" s="27" t="s">
         <v>3128</v>
       </c>
       <c r="B31" s="28"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>3122</v>
       </c>
@@ -59531,7 +59580,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="F22:G26">
+  <sortState ref="F23:G27">
     <sortCondition ref="G22"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>